<commit_message>
Cập nhật địa chỉ IP
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="IP-Planning" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="IP-Planning (2)" sheetId="3" r:id="rId3"/>
     <sheet name="IP-Planning CEPH" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet3" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="111">
   <si>
     <t>Controller</t>
   </si>
@@ -310,13 +311,84 @@
   </si>
   <si>
     <t>IP PLANNING FOR CEPH</t>
+  </si>
+  <si>
+    <t>CPU
+ (core)</t>
+  </si>
+  <si>
+    <t>RAM 
+(GB)</t>
+  </si>
+  <si>
+    <t>DATA DISK2
+(GB)</t>
+  </si>
+  <si>
+    <t>DATA DISK5
+(GB)</t>
+  </si>
+  <si>
+    <t>OS 
+DISK1
+(GB)</t>
+  </si>
+  <si>
+    <t>DATA DISK3
+(GB)</t>
+  </si>
+  <si>
+    <t>DATA DISK4
+(GB)</t>
+  </si>
+  <si>
+    <t>Inteface</t>
+  </si>
+  <si>
+    <t>DNS</t>
+  </si>
+  <si>
+    <t>eth3</t>
+  </si>
+  <si>
+    <t>8.8.8.8</t>
+  </si>
+  <si>
+    <t>RAM
+(GB)</t>
+  </si>
+  <si>
+    <t>DISK1
+(GB)</t>
+  </si>
+  <si>
+    <t>DISK5
+(GB)</t>
+  </si>
+  <si>
+    <t>DISK4
+(GB)</t>
+  </si>
+  <si>
+    <t>DISK3
+(GB)</t>
+  </si>
+  <si>
+    <t>DISK2
+(GB)</t>
+  </si>
+  <si>
+    <t>PHÂN HOẠCH CÁC ĐỊA CHỈ IP CHO MÁY CHỦ</t>
+  </si>
+  <si>
+    <t>YÊU CẦU TỐI THIỂU VỀ PHẦN CỨNG LAB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,8 +455,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,6 +500,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -723,7 +838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -844,6 +959,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -901,29 +1036,68 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,16 +1397,16 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="3:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
@@ -1281,7 +1455,7 @@
       </c>
     </row>
     <row r="7" spans="3:10" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="51" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -1307,7 +1481,7 @@
       </c>
     </row>
     <row r="8" spans="3:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="44"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="22" t="s">
         <v>3</v>
       </c>
@@ -1331,7 +1505,7 @@
       </c>
     </row>
     <row r="9" spans="3:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="45"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="24" t="s">
         <v>4</v>
       </c>
@@ -1355,7 +1529,7 @@
       </c>
     </row>
     <row r="10" spans="3:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="50" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -1381,7 +1555,7 @@
       </c>
     </row>
     <row r="11" spans="3:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="42"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="22" t="s">
         <v>3</v>
       </c>
@@ -1405,7 +1579,7 @@
       </c>
     </row>
     <row r="12" spans="3:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="42"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="24" t="s">
         <v>4</v>
       </c>
@@ -1477,7 +1651,7 @@
       </c>
     </row>
     <row r="15" spans="3:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="54" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="21" t="s">
@@ -1503,7 +1677,7 @@
       </c>
     </row>
     <row r="16" spans="3:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="47"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="23" t="s">
         <v>29</v>
       </c>
@@ -1527,7 +1701,7 @@
       </c>
     </row>
     <row r="17" spans="3:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="48"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="25" t="s">
         <v>31</v>
       </c>
@@ -1629,14 +1803,14 @@
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="53"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="54"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
     </row>
     <row r="7" spans="3:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="13" t="s">
@@ -1699,14 +1873,14 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="54"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="13" t="s">
@@ -1769,14 +1943,14 @@
       </c>
     </row>
     <row r="14" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="55" t="s">
+      <c r="C14" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="56"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="57"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="65"/>
     </row>
     <row r="15" spans="3:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="5"/>
@@ -1859,17 +2033,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
@@ -1947,7 +2121,7 @@
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="51" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -1985,7 +2159,7 @@
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="44"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="22" t="s">
         <v>3</v>
       </c>
@@ -2021,7 +2195,7 @@
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C9" s="45"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="24" t="s">
         <v>4</v>
       </c>
@@ -2057,7 +2231,7 @@
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="66" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -2095,7 +2269,7 @@
       </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="42"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="22" t="s">
         <v>3</v>
       </c>
@@ -2131,7 +2305,7 @@
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="42"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="24" t="s">
         <v>4</v>
       </c>
@@ -2167,7 +2341,7 @@
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="66" t="s">
         <v>55</v>
       </c>
       <c r="D13" s="20" t="s">
@@ -2197,7 +2371,7 @@
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C14" s="42"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="22" t="s">
         <v>3</v>
       </c>
@@ -2225,7 +2399,7 @@
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="42"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="24" t="s">
         <v>4</v>
       </c>
@@ -2325,7 +2499,7 @@
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="54" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -2363,7 +2537,7 @@
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="47"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="23" t="s">
         <v>29</v>
       </c>
@@ -2399,7 +2573,7 @@
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="48"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="25" t="s">
         <v>31</v>
       </c>
@@ -2511,17 +2685,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
@@ -2599,7 +2773,7 @@
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="51" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="20" t="s">
@@ -2637,7 +2811,7 @@
       </c>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C8" s="44"/>
+      <c r="C8" s="52"/>
       <c r="D8" s="22" t="s">
         <v>3</v>
       </c>
@@ -2673,7 +2847,7 @@
       </c>
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C9" s="45"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="24" t="s">
         <v>4</v>
       </c>
@@ -2709,7 +2883,7 @@
       </c>
     </row>
     <row r="10" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="66" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="20" t="s">
@@ -2747,7 +2921,7 @@
       </c>
     </row>
     <row r="11" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C11" s="42"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="22" t="s">
         <v>3</v>
       </c>
@@ -2783,7 +2957,7 @@
       </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="42"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="24" t="s">
         <v>4</v>
       </c>
@@ -2819,7 +2993,7 @@
       </c>
     </row>
     <row r="13" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="66" t="s">
         <v>55</v>
       </c>
       <c r="D13" s="20" t="s">
@@ -2849,7 +3023,7 @@
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C14" s="42"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="22" t="s">
         <v>3</v>
       </c>
@@ -2877,7 +3051,7 @@
       </c>
     </row>
     <row r="15" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C15" s="42"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="24" t="s">
         <v>4</v>
       </c>
@@ -2977,7 +3151,7 @@
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="54" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="21" t="s">
@@ -3015,7 +3189,7 @@
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="47"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="23" t="s">
         <v>29</v>
       </c>
@@ -3051,7 +3225,7 @@
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="48"/>
+      <c r="C20" s="56"/>
       <c r="D20" s="25" t="s">
         <v>31</v>
       </c>
@@ -3143,10 +3317,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F20"/>
+  <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3155,174 +3329,752 @@
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="66" t="s">
+    <row r="2" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C2" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="69"/>
-      <c r="C4" s="68" t="s">
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+    </row>
+    <row r="4" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="49"/>
+      <c r="C4" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="47" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="69"/>
-      <c r="C5" s="68" t="s">
+      <c r="G4" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="K4" s="71" t="s">
+        <v>97</v>
+      </c>
+      <c r="L4" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="49"/>
+      <c r="C5" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="65" t="s">
+      <c r="F5" s="46" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="69"/>
-      <c r="C6" s="68" t="s">
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+    </row>
+    <row r="6" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="49"/>
+      <c r="C6" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="65" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="69"/>
-      <c r="C7" s="68" t="s">
+      <c r="D6" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+    </row>
+    <row r="7" spans="2:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="49"/>
+      <c r="C7" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65" t="s">
+      <c r="D7" s="46"/>
+      <c r="E7" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="65"/>
-    </row>
-    <row r="9" spans="2:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C9" s="64"/>
-      <c r="D9" s="64" t="s">
+      <c r="F7" s="46"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+    </row>
+    <row r="9" spans="2:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C9" s="45"/>
+      <c r="D9" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="64" t="s">
+      <c r="E9" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="45" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C10" s="64" t="s">
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="70"/>
+    </row>
+    <row r="10" spans="2:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C10" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="45" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C11" s="64" t="s">
+      <c r="G10" s="72">
+        <v>4</v>
+      </c>
+      <c r="H10" s="45">
+        <v>2</v>
+      </c>
+      <c r="I10" s="45">
+        <v>40</v>
+      </c>
+      <c r="J10" s="45">
+        <v>60</v>
+      </c>
+      <c r="K10" s="45">
+        <v>60</v>
+      </c>
+      <c r="L10" s="45">
+        <v>60</v>
+      </c>
+      <c r="M10" s="45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C11" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="64" t="s">
+      <c r="E11" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="45" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C12" s="64" t="s">
+      <c r="G11" s="72">
+        <v>4</v>
+      </c>
+      <c r="H11" s="45">
+        <v>2</v>
+      </c>
+      <c r="I11" s="45">
+        <v>40</v>
+      </c>
+      <c r="J11" s="45">
+        <v>60</v>
+      </c>
+      <c r="K11" s="45">
+        <v>60</v>
+      </c>
+      <c r="L11" s="45">
+        <v>60</v>
+      </c>
+      <c r="M11" s="45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C12" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="45" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-    </row>
-    <row r="14" spans="2:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-    </row>
-    <row r="15" spans="2:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-    </row>
-    <row r="16" spans="2:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-    </row>
-    <row r="17" spans="3:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-    </row>
-    <row r="18" spans="3:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-    </row>
-    <row r="19" spans="3:6" s="61" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-    </row>
-    <row r="20" spans="3:6" s="61" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="G12" s="72">
+        <v>4</v>
+      </c>
+      <c r="H12" s="45">
+        <v>2</v>
+      </c>
+      <c r="I12" s="45">
+        <v>40</v>
+      </c>
+      <c r="J12" s="45">
+        <v>60</v>
+      </c>
+      <c r="K12" s="45">
+        <v>60</v>
+      </c>
+      <c r="L12" s="45">
+        <v>60</v>
+      </c>
+      <c r="M12" s="45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="70"/>
+      <c r="J13" s="70"/>
+      <c r="K13" s="70"/>
+      <c r="L13" s="70"/>
+      <c r="M13" s="70"/>
+    </row>
+    <row r="14" spans="2:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="70"/>
+      <c r="I14" s="70"/>
+      <c r="J14" s="70"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="70"/>
+      <c r="M14" s="70"/>
+    </row>
+    <row r="15" spans="2:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="70"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="70"/>
+    </row>
+    <row r="16" spans="2:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+    </row>
+    <row r="17" spans="3:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="70"/>
+      <c r="J17" s="70"/>
+      <c r="K17" s="70"/>
+      <c r="L17" s="70"/>
+      <c r="M17" s="70"/>
+    </row>
+    <row r="18" spans="3:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
+    </row>
+    <row r="19" spans="3:13" s="42" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+    </row>
+    <row r="20" spans="3:13" s="42" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="8">
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="M4:M7"/>
     <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G4:G7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="J4:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:N15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="15.7109375" style="73" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="73" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" style="73" customWidth="1"/>
+    <col min="6" max="7" width="15.7109375" style="73" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="73" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="73" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="9.5703125" style="73" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" s="42" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="87" t="s">
+        <v>110</v>
+      </c>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="89"/>
+    </row>
+    <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
+      <c r="B3" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="82" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" s="81" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="83" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" s="83" t="s">
+        <v>108</v>
+      </c>
+      <c r="L3" s="83" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" s="83" t="s">
+        <v>106</v>
+      </c>
+      <c r="N3" s="83" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="90" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="74">
+        <v>4</v>
+      </c>
+      <c r="I4" s="74">
+        <v>2</v>
+      </c>
+      <c r="J4" s="79">
+        <v>40</v>
+      </c>
+      <c r="K4" s="80">
+        <v>60</v>
+      </c>
+      <c r="L4" s="80">
+        <v>60</v>
+      </c>
+      <c r="M4" s="80">
+        <v>60</v>
+      </c>
+      <c r="N4" s="80">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="91"/>
+      <c r="C5" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="77" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="91"/>
+      <c r="C6" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="92"/>
+      <c r="C7" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="79"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
+      <c r="M7" s="80"/>
+      <c r="N7" s="80"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="90" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="74">
+        <v>4</v>
+      </c>
+      <c r="I8" s="74">
+        <v>2</v>
+      </c>
+      <c r="J8" s="79">
+        <v>40</v>
+      </c>
+      <c r="K8" s="80">
+        <v>60</v>
+      </c>
+      <c r="L8" s="80">
+        <v>60</v>
+      </c>
+      <c r="M8" s="80">
+        <v>60</v>
+      </c>
+      <c r="N8" s="80">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="91"/>
+      <c r="C9" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="77" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="91"/>
+      <c r="C10" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="80"/>
+      <c r="N10" s="80"/>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="92"/>
+      <c r="C11" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+      <c r="M11" s="80"/>
+      <c r="N11" s="80"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="90" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="74">
+        <v>4</v>
+      </c>
+      <c r="I12" s="74">
+        <v>2</v>
+      </c>
+      <c r="J12" s="79">
+        <v>40</v>
+      </c>
+      <c r="K12" s="80">
+        <v>60</v>
+      </c>
+      <c r="L12" s="80">
+        <v>60</v>
+      </c>
+      <c r="M12" s="80">
+        <v>60</v>
+      </c>
+      <c r="N12" s="80">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="91"/>
+      <c r="C13" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="77" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="77" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="80"/>
+      <c r="M13" s="80"/>
+      <c r="N13" s="80"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="91"/>
+      <c r="C14" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="78" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="78" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="80"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="92"/>
+      <c r="C15" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="79"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="80"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="M8:M11"/>
+    <mergeCell ref="N8:N11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="J8:J11"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cập nhật ip planning
</commit_message>
<xml_diff>
--- a/tools/IP-Planning-Hardware-Requirements.xlsx
+++ b/tools/IP-Planning-Hardware-Requirements.xlsx
@@ -1062,6 +1062,24 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1078,24 +1096,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3672,7 +3672,7 @@
   <dimension ref="B2:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B12" sqref="B12:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3688,23 +3688,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" s="42" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="84" t="s">
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="90" t="s">
         <v>110</v>
       </c>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="86"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="92"/>
     </row>
     <row r="3" spans="2:14" ht="33" x14ac:dyDescent="0.25">
       <c r="B3" s="58" t="s">
@@ -3748,7 +3748,7 @@
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="83" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="45" t="s">
@@ -3762,30 +3762,30 @@
       </c>
       <c r="F4" s="54"/>
       <c r="G4" s="54"/>
-      <c r="H4" s="91">
+      <c r="H4" s="82">
         <v>4</v>
       </c>
-      <c r="I4" s="91">
-        <v>2</v>
-      </c>
-      <c r="J4" s="92">
+      <c r="I4" s="82">
+        <v>2</v>
+      </c>
+      <c r="J4" s="86">
         <v>40</v>
       </c>
-      <c r="K4" s="87">
+      <c r="K4" s="81">
         <v>60</v>
       </c>
-      <c r="L4" s="87">
+      <c r="L4" s="81">
         <v>60</v>
       </c>
-      <c r="M4" s="87">
+      <c r="M4" s="81">
         <v>60</v>
       </c>
-      <c r="N4" s="87">
+      <c r="N4" s="81">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="89"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="45" t="s">
         <v>5</v>
       </c>
@@ -3801,16 +3801,16 @@
       <c r="G5" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="87"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="81"/>
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="89"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="45" t="s">
         <v>90</v>
       </c>
@@ -3822,16 +3822,16 @@
       </c>
       <c r="F6" s="56"/>
       <c r="G6" s="56"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="87"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="90"/>
+      <c r="B7" s="85"/>
       <c r="C7" s="45" t="s">
         <v>101</v>
       </c>
@@ -3839,16 +3839,16 @@
       <c r="E7" s="53"/>
       <c r="F7" s="53"/>
       <c r="G7" s="53"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="88" t="s">
+      <c r="B8" s="83" t="s">
         <v>66</v>
       </c>
       <c r="C8" s="45" t="s">
@@ -3862,30 +3862,30 @@
       </c>
       <c r="F8" s="54"/>
       <c r="G8" s="54"/>
-      <c r="H8" s="91">
+      <c r="H8" s="82">
         <v>4</v>
       </c>
-      <c r="I8" s="91">
-        <v>2</v>
-      </c>
-      <c r="J8" s="92">
+      <c r="I8" s="82">
+        <v>2</v>
+      </c>
+      <c r="J8" s="86">
         <v>40</v>
       </c>
-      <c r="K8" s="87">
+      <c r="K8" s="81">
         <v>60</v>
       </c>
-      <c r="L8" s="87">
+      <c r="L8" s="81">
         <v>60</v>
       </c>
-      <c r="M8" s="87">
+      <c r="M8" s="81">
         <v>60</v>
       </c>
-      <c r="N8" s="87">
+      <c r="N8" s="81">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="89"/>
+      <c r="B9" s="84"/>
       <c r="C9" s="45" t="s">
         <v>5</v>
       </c>
@@ -3901,16 +3901,16 @@
       <c r="G9" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="H9" s="91"/>
-      <c r="I9" s="91"/>
-      <c r="J9" s="92"/>
-      <c r="K9" s="87"/>
-      <c r="L9" s="87"/>
-      <c r="M9" s="87"/>
-      <c r="N9" s="87"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="89"/>
+      <c r="B10" s="84"/>
       <c r="C10" s="45" t="s">
         <v>90</v>
       </c>
@@ -3922,16 +3922,16 @@
       </c>
       <c r="F10" s="56"/>
       <c r="G10" s="56"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="91"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="87"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="87"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="90"/>
+      <c r="B11" s="85"/>
       <c r="C11" s="45" t="s">
         <v>101</v>
       </c>
@@ -3939,17 +3939,17 @@
       <c r="E11" s="53"/>
       <c r="F11" s="53"/>
       <c r="G11" s="53"/>
-      <c r="H11" s="91"/>
-      <c r="I11" s="91"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="87"/>
-      <c r="L11" s="87"/>
-      <c r="M11" s="87"/>
-      <c r="N11" s="87"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="81"/>
+      <c r="L11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="88" t="s">
-        <v>66</v>
+      <c r="B12" s="83" t="s">
+        <v>67</v>
       </c>
       <c r="C12" s="45" t="s">
         <v>1</v>
@@ -3962,30 +3962,30 @@
       </c>
       <c r="F12" s="54"/>
       <c r="G12" s="54"/>
-      <c r="H12" s="91">
+      <c r="H12" s="82">
         <v>4</v>
       </c>
-      <c r="I12" s="91">
-        <v>2</v>
-      </c>
-      <c r="J12" s="92">
+      <c r="I12" s="82">
+        <v>2</v>
+      </c>
+      <c r="J12" s="86">
         <v>40</v>
       </c>
-      <c r="K12" s="87">
+      <c r="K12" s="81">
         <v>60</v>
       </c>
-      <c r="L12" s="87">
+      <c r="L12" s="81">
         <v>60</v>
       </c>
-      <c r="M12" s="87">
+      <c r="M12" s="81">
         <v>60</v>
       </c>
-      <c r="N12" s="87">
+      <c r="N12" s="81">
         <v>60</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="89"/>
+      <c r="B13" s="84"/>
       <c r="C13" s="45" t="s">
         <v>5</v>
       </c>
@@ -4001,16 +4001,16 @@
       <c r="G13" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="H13" s="91"/>
-      <c r="I13" s="91"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="87"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="87"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="89"/>
+      <c r="B14" s="84"/>
       <c r="C14" s="45" t="s">
         <v>90</v>
       </c>
@@ -4022,16 +4022,16 @@
       </c>
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
-      <c r="H14" s="91"/>
-      <c r="I14" s="91"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="87"/>
-      <c r="L14" s="87"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="87"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="81"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="90"/>
+      <c r="B15" s="85"/>
       <c r="C15" s="45" t="s">
         <v>101</v>
       </c>
@@ -4039,35 +4039,16 @@
       <c r="E15" s="53"/>
       <c r="F15" s="53"/>
       <c r="G15" s="53"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="87"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="87"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="M4:M7"/>
-    <mergeCell ref="N4:N7"/>
-    <mergeCell ref="I4:I7"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="K8:K11"/>
-    <mergeCell ref="L8:L11"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="J4:J7"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="L4:L7"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:N2"/>
-    <mergeCell ref="M8:M11"/>
-    <mergeCell ref="N8:N11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
@@ -4075,6 +4056,25 @@
     <mergeCell ref="H8:H11"/>
     <mergeCell ref="I8:I11"/>
     <mergeCell ref="J8:J11"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="J4:J7"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="L4:L7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:N2"/>
+    <mergeCell ref="M4:M7"/>
+    <mergeCell ref="N4:N7"/>
+    <mergeCell ref="I4:I7"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="K8:K11"/>
+    <mergeCell ref="L8:L11"/>
+    <mergeCell ref="M8:M11"/>
+    <mergeCell ref="N8:N11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>